<commit_message>
fixed bug in merge_by
</commit_message>
<xml_diff>
--- a/nn128_50k_samples.xlsx
+++ b/nn128_50k_samples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t xml:space="preserve">sample</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">merged_sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pulse</t>
   </si>
   <si>
     <t xml:space="preserve">50k_1_1__A</t>
@@ -213,10 +219,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -243,16 +249,22 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>300</v>
@@ -264,16 +276,24 @@
         <f aca="false">LEFT(A2, 7)</f>
         <v>50k_1_1</v>
       </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">RIGHT(A2, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A2, 4), 1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>300</v>
@@ -285,16 +305,24 @@
         <f aca="false">LEFT(A3, 7)</f>
         <v>50k_1_1</v>
       </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">RIGHT(A3, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A3, 4), 1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>300</v>
@@ -306,16 +334,24 @@
         <f aca="false">LEFT(A4, 7)</f>
         <v>50k_1_2</v>
       </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">RIGHT(A4, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A4, 4), 1)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>300</v>
@@ -327,16 +363,24 @@
         <f aca="false">LEFT(A5, 7)</f>
         <v>50k_1_2</v>
       </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">RIGHT(A5, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A5, 4), 1)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>300</v>
@@ -348,16 +392,24 @@
         <f aca="false">LEFT(A6, 7)</f>
         <v>50k_2_1</v>
       </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">RIGHT(A6, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A6, 4), 1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>300</v>
@@ -369,16 +421,24 @@
         <f aca="false">LEFT(A7, 7)</f>
         <v>50k_2_1</v>
       </c>
+      <c r="G7" s="0" t="str">
+        <f aca="false">RIGHT(A7, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A7, 4), 1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>300</v>
@@ -390,16 +450,24 @@
         <f aca="false">LEFT(A8, 7)</f>
         <v>50k_2_2</v>
       </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">RIGHT(A8, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="H8" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A8, 4), 1)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>300</v>
@@ -411,16 +479,24 @@
         <f aca="false">LEFT(A9, 7)</f>
         <v>50k_2_2</v>
       </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">RIGHT(A9, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A9, 4), 1)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>300</v>
@@ -432,16 +508,24 @@
         <f aca="false">LEFT(A10, 7)</f>
         <v>50k_3_1</v>
       </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">RIGHT(A10, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="H10" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A10, 4), 1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>300</v>
@@ -453,16 +537,24 @@
         <f aca="false">LEFT(A11, 7)</f>
         <v>50k_3_1</v>
       </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">RIGHT(A11, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="H11" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A11, 4), 1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>300</v>
@@ -474,16 +566,24 @@
         <f aca="false">LEFT(A12, 7)</f>
         <v>50k_3_2</v>
       </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">RIGHT(A12, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A12, 4), 1)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>300</v>
@@ -494,6 +594,14 @@
       <c r="F13" s="1" t="str">
         <f aca="false">LEFT(A13, 7)</f>
         <v>50k_3_2</v>
+      </c>
+      <c r="G13" s="0" t="str">
+        <f aca="false">RIGHT(A13, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="H13" s="0" t="str">
+        <f aca="false">LEFT(RIGHT(A13, 4), 1)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added min_flip_dist and run_markov
</commit_message>
<xml_diff>
--- a/nn128_50k_samples.xlsx
+++ b/nn128_50k_samples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t xml:space="preserve">sample</t>
   </si>
@@ -35,15 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">min_r2_len</t>
-  </si>
-  <si>
-    <t xml:space="preserve">merged_sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pulse</t>
   </si>
   <si>
     <t xml:space="preserve">50k_1_1__A</t>
@@ -219,10 +210,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -246,25 +237,17 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>300</v>
@@ -272,28 +255,17 @@
       <c r="E2" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F2" s="1" t="str">
-        <f aca="false">LEFT(A2, 7)</f>
-        <v>50k_1_1</v>
-      </c>
-      <c r="G2" s="0" t="str">
-        <f aca="false">RIGHT(A2, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="H2" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A2, 4), 1)</f>
-        <v>1</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>300</v>
@@ -301,28 +273,17 @@
       <c r="E3" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F3" s="1" t="str">
-        <f aca="false">LEFT(A3, 7)</f>
-        <v>50k_1_1</v>
-      </c>
-      <c r="G3" s="0" t="str">
-        <f aca="false">RIGHT(A3, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="H3" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A3, 4), 1)</f>
-        <v>1</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>300</v>
@@ -330,28 +291,17 @@
       <c r="E4" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F4" s="1" t="str">
-        <f aca="false">LEFT(A4, 7)</f>
-        <v>50k_1_2</v>
-      </c>
-      <c r="G4" s="0" t="str">
-        <f aca="false">RIGHT(A4, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="H4" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A4, 4), 1)</f>
-        <v>2</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>300</v>
@@ -359,28 +309,17 @@
       <c r="E5" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F5" s="1" t="str">
-        <f aca="false">LEFT(A5, 7)</f>
-        <v>50k_1_2</v>
-      </c>
-      <c r="G5" s="0" t="str">
-        <f aca="false">RIGHT(A5, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="H5" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A5, 4), 1)</f>
-        <v>2</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>300</v>
@@ -388,28 +327,17 @@
       <c r="E6" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F6" s="1" t="str">
-        <f aca="false">LEFT(A6, 7)</f>
-        <v>50k_2_1</v>
-      </c>
-      <c r="G6" s="0" t="str">
-        <f aca="false">RIGHT(A6, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="H6" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A6, 4), 1)</f>
-        <v>1</v>
-      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>300</v>
@@ -417,28 +345,17 @@
       <c r="E7" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F7" s="1" t="str">
-        <f aca="false">LEFT(A7, 7)</f>
-        <v>50k_2_1</v>
-      </c>
-      <c r="G7" s="0" t="str">
-        <f aca="false">RIGHT(A7, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="H7" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A7, 4), 1)</f>
-        <v>1</v>
-      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>300</v>
@@ -446,28 +363,17 @@
       <c r="E8" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F8" s="1" t="str">
-        <f aca="false">LEFT(A8, 7)</f>
-        <v>50k_2_2</v>
-      </c>
-      <c r="G8" s="0" t="str">
-        <f aca="false">RIGHT(A8, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="H8" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A8, 4), 1)</f>
-        <v>2</v>
-      </c>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>300</v>
@@ -475,28 +381,17 @@
       <c r="E9" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F9" s="1" t="str">
-        <f aca="false">LEFT(A9, 7)</f>
-        <v>50k_2_2</v>
-      </c>
-      <c r="G9" s="0" t="str">
-        <f aca="false">RIGHT(A9, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="H9" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A9, 4), 1)</f>
-        <v>2</v>
-      </c>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>300</v>
@@ -504,28 +399,17 @@
       <c r="E10" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F10" s="1" t="str">
-        <f aca="false">LEFT(A10, 7)</f>
-        <v>50k_3_1</v>
-      </c>
-      <c r="G10" s="0" t="str">
-        <f aca="false">RIGHT(A10, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="H10" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A10, 4), 1)</f>
-        <v>1</v>
-      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>300</v>
@@ -533,28 +417,17 @@
       <c r="E11" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F11" s="1" t="str">
-        <f aca="false">LEFT(A11, 7)</f>
-        <v>50k_3_1</v>
-      </c>
-      <c r="G11" s="0" t="str">
-        <f aca="false">RIGHT(A11, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="H11" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A11, 4), 1)</f>
-        <v>1</v>
-      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>300</v>
@@ -562,28 +435,17 @@
       <c r="E12" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F12" s="1" t="str">
-        <f aca="false">LEFT(A12, 7)</f>
-        <v>50k_3_2</v>
-      </c>
-      <c r="G12" s="0" t="str">
-        <f aca="false">RIGHT(A12, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="H12" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A12, 4), 1)</f>
-        <v>2</v>
-      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>300</v>
@@ -591,18 +453,7 @@
       <c r="E13" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F13" s="1" t="str">
-        <f aca="false">LEFT(A13, 7)</f>
-        <v>50k_3_2</v>
-      </c>
-      <c r="G13" s="0" t="str">
-        <f aca="false">RIGHT(A13, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="H13" s="0" t="str">
-        <f aca="false">LEFT(RIGHT(A13, 4), 1)</f>
-        <v>2</v>
-      </c>
+      <c r="F13" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>